<commit_message>
remove unirx , fix firebase check, build for ios,
</commit_message>
<xml_diff>
--- a/DestroyViruses/Assets/Tables/TableLanguage.xlsx
+++ b/DestroyViruses/Assets/Tables/TableLanguage.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578">
   <si>
     <t>id</t>
   </si>
@@ -1613,6 +1613,15 @@
     <t>商店5</t>
   </si>
   <si>
+    <t>Shop_vip</t>
+  </si>
+  <si>
+    <t>vip</t>
+  </si>
+  <si>
+    <t>VIP</t>
+  </si>
+  <si>
     <t>Shop_price1</t>
   </si>
   <si>
@@ -1656,6 +1665,12 @@
   </si>
   <si>
     <t>$39.99</t>
+  </si>
+  <si>
+    <t>Shop_vip_price</t>
+  </si>
+  <si>
+    <t>$1.99</t>
   </si>
   <si>
     <t>vipDisclaimer</t>
@@ -1753,9 +1768,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -1820,34 +1835,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1856,6 +1847,14 @@
       <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1877,7 +1876,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1891,10 +1913,18 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1906,25 +1936,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1956,13 +1971,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1974,13 +1989,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1998,7 +2013,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2010,25 +2061,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2040,7 +2085,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2052,67 +2115,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2124,7 +2139,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2147,26 +2162,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2178,6 +2173,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2197,17 +2201,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2227,6 +2227,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2238,124 +2253,124 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2364,13 +2379,13 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2763,10 +2778,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:D202"/>
+  <dimension ref="A1:D204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="D185" sqref="D185:D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" outlineLevelCol="3"/>
@@ -5365,102 +5380,130 @@
         <v>544</v>
       </c>
     </row>
-    <row r="196" ht="333" customHeight="1" spans="1:4">
-      <c r="A196" s="1" t="s">
+    <row r="195" spans="1:4">
+      <c r="A195" s="10" t="s">
         <v>545</v>
       </c>
+      <c r="B195" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>547</v>
+      </c>
+      <c r="D195" s="10" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4">
+      <c r="A196" s="10" t="s">
+        <v>548</v>
+      </c>
       <c r="B196" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="C196" s="11" t="s">
-        <v>547</v>
-      </c>
-      <c r="D196" s="11" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="197" s="1" customFormat="1" spans="1:4">
-      <c r="A197" s="1" t="s">
+        <v>531</v>
+      </c>
+      <c r="C196" s="10" t="s">
         <v>549</v>
       </c>
-      <c r="B197" s="1" t="s">
+      <c r="D196" s="10" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="198" ht="333" customHeight="1" spans="1:4">
+      <c r="A198" s="1" t="s">
         <v>550</v>
       </c>
-      <c r="C197" s="12" t="s">
+      <c r="B198" s="1" t="s">
         <v>551</v>
       </c>
-      <c r="D197" s="12" t="s">
+      <c r="C198" s="11" t="s">
         <v>552</v>
       </c>
-    </row>
-    <row r="198" s="1" customFormat="1" spans="1:4">
-      <c r="A198" s="1" t="s">
+      <c r="D198" s="11" t="s">
         <v>553</v>
-      </c>
-      <c r="B198" s="1" t="s">
-        <v>554</v>
-      </c>
-      <c r="C198" s="12" t="s">
-        <v>555</v>
-      </c>
-      <c r="D198" s="12" t="s">
-        <v>556</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="1" spans="1:4">
       <c r="A199" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="C199" s="12" t="s">
+        <v>556</v>
+      </c>
+      <c r="D199" s="12" t="s">
         <v>557</v>
-      </c>
-      <c r="B199" s="1" t="s">
-        <v>558</v>
-      </c>
-      <c r="C199" s="12" t="s">
-        <v>559</v>
-      </c>
-      <c r="D199" s="12" t="s">
-        <v>560</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="1" spans="1:4">
       <c r="A200" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="C200" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="D200" s="12" t="s">
         <v>561</v>
-      </c>
-      <c r="B200" s="1" t="s">
-        <v>562</v>
-      </c>
-      <c r="C200" s="12" t="s">
-        <v>563</v>
-      </c>
-      <c r="D200" s="12" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="1" spans="1:4">
       <c r="A201" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="C201" s="12" t="s">
+        <v>564</v>
+      </c>
+      <c r="D201" s="12" t="s">
         <v>565</v>
       </c>
-      <c r="B201" s="1" t="s">
+    </row>
+    <row r="202" s="1" customFormat="1" spans="1:4">
+      <c r="A202" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="C201" s="12" t="s">
+      <c r="B202" s="1" t="s">
         <v>567</v>
       </c>
-      <c r="D201" s="12" t="s">
+      <c r="C202" s="12" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="202" spans="1:4">
-      <c r="A202" s="1" t="s">
+      <c r="D202" s="12" t="s">
         <v>569</v>
       </c>
-      <c r="B202" s="1" t="s">
+    </row>
+    <row r="203" s="1" customFormat="1" spans="1:4">
+      <c r="A203" s="1" t="s">
         <v>570</v>
       </c>
-      <c r="C202" s="12" t="s">
+      <c r="B203" s="1" t="s">
         <v>571</v>
       </c>
-      <c r="D202" s="12" t="s">
+      <c r="C203" s="12" t="s">
         <v>572</v>
+      </c>
+      <c r="D203" s="12" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4">
+      <c r="A204" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B204" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C204" s="12" t="s">
+        <v>576</v>
+      </c>
+      <c r="D204" s="12" t="s">
+        <v>577</v>
       </c>
     </row>
   </sheetData>

</xml_diff>